<commit_message>
updated script and schema
</commit_message>
<xml_diff>
--- a/OldEgg Schema.xlsx
+++ b/OldEgg Schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/irfansyakir/Documents/OldEgg Project/OldEgg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E2F7F6-41DD-BE4E-934D-D98282AAC711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCDD31E-FE23-5B43-A304-11FD76767DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{77102896-566B-D147-AF31-283E502716C7}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="216">
   <si>
     <t>link</t>
   </si>
@@ -74,18 +74,12 @@
     <t>https://media.ldlc.com/r1600/ld/products/00/05/98/55/LD0005985556.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">	LGA1700</t>
-  </si>
-  <si>
     <t>https://www.asrock.com/mb/photo/B660M-HDV(M1).png</t>
   </si>
   <si>
     <t>https://simlimsquare.com.sg/image/images/620da7ae93efb.jpg?p=full</t>
   </si>
   <si>
-    <t xml:space="preserve">	LGA1200</t>
-  </si>
-  <si>
     <t>https://m.media-amazon.com/images/I/91+aWDgEKYL.jpg</t>
   </si>
   <si>
@@ -476,36 +470,6 @@
     <t xml:space="preserve">NVIDIA MSI RTX 2070 SUPER VENTUS </t>
   </si>
   <si>
-    <t>GIGABYTE RX 6500XT EAGLE</t>
-  </si>
-  <si>
-    <t>MSI RX 6650XT MECH</t>
-  </si>
-  <si>
-    <t>AMD RYZEN 7 5800X3D</t>
-  </si>
-  <si>
-    <t>AMD RYZEN 7 5600X</t>
-  </si>
-  <si>
-    <t>AMD RYZEN 7 5800X</t>
-  </si>
-  <si>
-    <t>AMD RYZEN 9 7950X</t>
-  </si>
-  <si>
-    <t>INTEL CORE i5-13600K</t>
-  </si>
-  <si>
-    <t>INTEL CORE i9-13900K</t>
-  </si>
-  <si>
-    <t>INTEL CORE i7-12700KF</t>
-  </si>
-  <si>
-    <t>AMD RYZEN 9 5900X</t>
-  </si>
-  <si>
     <t>https://m.media-amazon.com/images/I/61Kq99IRdcL.jpg</t>
   </si>
   <si>
@@ -566,15 +530,9 @@
     <t>https://m.media-amazon.com/images/I/91ZpekDlH3L._AC_SL1500_.jpg</t>
   </si>
   <si>
-    <t>XFX SPEEDSTER MERC310 AMD Radeon RX 7900XT</t>
-  </si>
-  <si>
     <t>https://m.media-amazon.com/images/I/61F2rF1rKCL._AC_UL640_FMwebp_QL65_.jpg</t>
   </si>
   <si>
-    <t>ASUS TUF GAMING RTX 4080</t>
-  </si>
-  <si>
     <t>https://m.media-amazon.com/images/I/81BTQB6jbXL._AC_UL640_FMwebp_QL65_.jpg</t>
   </si>
   <si>
@@ -584,33 +542,160 @@
     <t>https://m.media-amazon.com/images/I/71AAVqtFfvL._AC_UL640_QL65_.jpg</t>
   </si>
   <si>
-    <t>MSI RTX 3060 GAMING X TRIO</t>
-  </si>
-  <si>
-    <t>ZOTAC GTX 1660 SUPER</t>
-  </si>
-  <si>
-    <t>GIGABYTE RX 6900 XT GAMING OC</t>
-  </si>
-  <si>
-    <t>https://m.media-amazon.com/images/I/811sBakp3+L._AC_UL640_FMwebp_QL65_.jpg</t>
-  </si>
-  <si>
-    <t>MSI GTX 1660 SUPER VENTUS XS</t>
-  </si>
-  <si>
     <t>https://m.media-amazon.com/images/I/619Ui9f--pL._AC_SL1000_.jpg</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 7 5800X3D</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 7 5600X</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 7 5800X</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 9 7950X</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 9 5900X</t>
+  </si>
+  <si>
+    <t>LGA1200</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/71XcVOdHX+S._AC_UY436_FMwebp_QL65_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/81ywJlcuVOL._AC_UY436_FMwebp_QL65_.jpg</t>
+  </si>
+  <si>
+    <t>AMD GIGABYTE RX 6500XT EAGLE</t>
+  </si>
+  <si>
+    <t>AMD MSI RX 6650XT MECH</t>
+  </si>
+  <si>
+    <t>AMD XFX SPEEDSTER MERC310 AMD RX 7900 XT</t>
+  </si>
+  <si>
+    <t>NVIDIA ASUS TUF GAMING RTX 4080</t>
+  </si>
+  <si>
+    <t>AMD GIGABYTE RX 6900 XT GAMING OC</t>
+  </si>
+  <si>
+    <t>NVIDIA ZOTAC GTX 1660 SUPER</t>
+  </si>
+  <si>
+    <t>NVIDIA MSI GTX 1660 SUPER VENTUS XS</t>
+  </si>
+  <si>
+    <t>NVIDIA GIGABYTE RTX 3070 GAMING OC</t>
+  </si>
+  <si>
+    <t>NVIDIA ZOTAC RTX 4070 TI TRINITY OC</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 5 5600G</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/51f2hkWjTlL._AC_UY436_FMwebp_QL65_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/41MO1qkT+FL._AC_UY436_FMwebp_QL65_.jpg</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 3 3200G</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/51Dx39HJ8kL._AC_UY436_FMwebp_QL65_.jpg</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 3 3100</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/71DTUOZdDnL._AC_UY436_FMwebp_QL65_.jpg</t>
+  </si>
+  <si>
+    <t>Intel Core i3-10100</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/51S2a+GyxUS._AC_UY436_FMwebp_QL65_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/51V+MalhMHL._AC_UY436_FMwebp_QL65_.jpg</t>
+  </si>
+  <si>
+    <t>Intel Core i5-12400</t>
+  </si>
+  <si>
+    <t>Intel Core i5-11400F</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/71LIKeM7GGL._AC_UY436_FMwebp_QL65_.jpg</t>
+  </si>
+  <si>
+    <t>Intel Core i5-13600K</t>
+  </si>
+  <si>
+    <t>Intel Core i9-13900K</t>
+  </si>
+  <si>
+    <t>Intel Core i7-12700KF</t>
+  </si>
+  <si>
+    <t>Intel Core i7-13700K</t>
+  </si>
+  <si>
+    <t>Intel Core i3-12100F</t>
+  </si>
+  <si>
+    <t>Intel Core i9-12900KF</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/510jsZcyEDL._AC_UY436_FMwebp_QL65_.jpg</t>
+  </si>
+  <si>
+    <t>Intel Core i9-11900K</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/71diouNMRHL._AC_UY436_FMwebp_QL65_.jpg</t>
+  </si>
+  <si>
+    <t>MSI MPG Z790 Edge WiFi DDR4</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/81LHT-z5-EL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASUS AM4 TUF Gaming X570-Plus (Wi-Fi) </t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/710hyHWebnL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/811WsAtV8FL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Asus ROG MAXIMUS Z690 HERO EVA(ROG x Evangelion)</t>
+  </si>
+  <si>
+    <t>NVIDIA ASUS ROG STRIX RTX 3080 EVA</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/81h5R6ojhwL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>https://dlcdnwebimgs.asus.com/gain/A96FC491-FEAA-4DFA-96A8-B95832F87C8B/w1000/h732</t>
+  </si>
+  <si>
+    <t>NVIDIA ASUS ROG STRIX RTX 3080 GUNDAM EDITON</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -661,11 +746,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -983,28 +1065,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FFAAB6F-9E62-3845-85E0-19A3456B57F7}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
         <v>115</v>
       </c>
-      <c r="B1" t="s">
-        <v>117</v>
-      </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1012,77 +1094,77 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B2" s="1">
+        <v>140</v>
+      </c>
+      <c r="B2">
         <v>1000</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>16</v>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B3" s="1">
+        <v>141</v>
+      </c>
+      <c r="B3">
         <v>700</v>
       </c>
       <c r="C3">
         <v>54</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>17</v>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B4" s="2">
+        <v>134</v>
+      </c>
+      <c r="B4">
         <v>2581.54</v>
       </c>
       <c r="C4">
         <v>15</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>18</v>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1923.52</v>
+        <v>139</v>
+      </c>
+      <c r="B5">
+        <v>1924</v>
       </c>
       <c r="C5">
         <v>18</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>19</v>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B6" s="3">
+        <v>135</v>
+      </c>
+      <c r="B6">
         <v>330</v>
       </c>
       <c r="C6">
         <v>88</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>20</v>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B7">
         <v>1200</v>
@@ -1090,13 +1172,13 @@
       <c r="C7">
         <v>55</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>21</v>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B8">
         <v>1100</v>
@@ -1104,13 +1186,13 @@
       <c r="C8">
         <v>96</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>22</v>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>175</v>
       </c>
       <c r="B9">
         <v>220</v>
@@ -1118,13 +1200,13 @@
       <c r="C9">
         <v>27</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>23</v>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>176</v>
       </c>
       <c r="B10">
         <v>451.64</v>
@@ -1132,13 +1214,13 @@
       <c r="C10">
         <v>31</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>24</v>
+      <c r="D10" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B11">
         <v>1262.76</v>
@@ -1147,12 +1229,12 @@
         <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B12">
         <v>2128</v>
@@ -1161,12 +1243,12 @@
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B13">
         <v>1488</v>
@@ -1175,12 +1257,12 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B14">
         <v>362.07</v>
@@ -1189,26 +1271,26 @@
         <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>180</v>
+        <v>215</v>
       </c>
       <c r="B15">
-        <v>603.44000000000005</v>
+        <v>1500</v>
       </c>
       <c r="C15">
         <v>27</v>
       </c>
-      <c r="D15" t="s">
-        <v>183</v>
+      <c r="D15" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B16">
         <v>384.44</v>
@@ -1217,7 +1299,49 @@
         <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>185</v>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>182</v>
+      </c>
+      <c r="B17">
+        <v>768.44</v>
+      </c>
+      <c r="C17">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>183</v>
+      </c>
+      <c r="B18">
+        <v>1145.55</v>
+      </c>
+      <c r="C18">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>212</v>
+      </c>
+      <c r="B19">
+        <v>1400</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -1231,18 +1355,20 @@
     <hyperlink ref="D8" r:id="rId7" xr:uid="{95A950B6-ADE6-4B04-A23A-14303BD71398}"/>
     <hyperlink ref="D9" r:id="rId8" xr:uid="{892B6719-E8BD-451D-81F4-60F8452A8CE5}"/>
     <hyperlink ref="D10" r:id="rId9" xr:uid="{9F622F1B-2533-4F95-94F3-9F0A5A1BF156}"/>
+    <hyperlink ref="D15" r:id="rId10" xr:uid="{0627D37E-1E17-C14F-A7F3-A91730F3AF53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDEF267F-2EC0-D449-8DB3-8973D99C4ABE}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView zoomScale="164" zoomScaleNormal="265" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" sqref="A1:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1252,13 +1378,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
         <v>115</v>
       </c>
-      <c r="B1" t="s">
-        <v>117</v>
-      </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1266,7 +1392,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="B2">
         <v>550</v>
@@ -1274,13 +1400,13 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>154</v>
+      <c r="D2" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="B3">
         <v>290.17</v>
@@ -1288,13 +1414,13 @@
       <c r="C3">
         <v>53</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>155</v>
+      <c r="D3" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="B4">
         <v>382.31</v>
@@ -1302,13 +1428,13 @@
       <c r="C4">
         <v>29</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>155</v>
+      <c r="D4" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>197</v>
       </c>
       <c r="B5">
         <v>492.47</v>
@@ -1316,13 +1442,13 @@
       <c r="C5">
         <v>35</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>156</v>
+      <c r="D5" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>198</v>
       </c>
       <c r="B6">
         <v>892</v>
@@ -1330,13 +1456,13 @@
       <c r="C6">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>157</v>
+      <c r="D6" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="B7">
         <v>921.23</v>
@@ -1344,13 +1470,13 @@
       <c r="C7">
         <v>13</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>158</v>
+      <c r="D7" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>199</v>
       </c>
       <c r="B8">
         <v>443.95</v>
@@ -1358,13 +1484,13 @@
       <c r="C8">
         <v>23</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>159</v>
+      <c r="D8" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>200</v>
       </c>
       <c r="B9">
         <v>643.37</v>
@@ -1372,13 +1498,13 @@
       <c r="C9">
         <v>34</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>160</v>
+      <c r="D9" s="1" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="B10">
         <v>538.91</v>
@@ -1386,8 +1512,134 @@
       <c r="C10">
         <v>199</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>161</v>
+      <c r="D10" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B11">
+        <v>177.69</v>
+      </c>
+      <c r="C11">
+        <v>515</v>
+      </c>
+      <c r="D11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>201</v>
+      </c>
+      <c r="B12">
+        <v>147.33000000000001</v>
+      </c>
+      <c r="C12">
+        <v>368</v>
+      </c>
+      <c r="D12" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>187</v>
+      </c>
+      <c r="B13">
+        <v>143.29</v>
+      </c>
+      <c r="C13">
+        <v>306</v>
+      </c>
+      <c r="D13" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>189</v>
+      </c>
+      <c r="B14">
+        <v>192.88</v>
+      </c>
+      <c r="C14">
+        <v>228</v>
+      </c>
+      <c r="D14" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>191</v>
+      </c>
+      <c r="B15">
+        <v>136.04</v>
+      </c>
+      <c r="C15">
+        <v>97</v>
+      </c>
+      <c r="D15" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B16">
+        <v>251.85</v>
+      </c>
+      <c r="C16">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>195</v>
+      </c>
+      <c r="B17">
+        <v>180.2</v>
+      </c>
+      <c r="C17">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>202</v>
+      </c>
+      <c r="B18">
+        <v>563.32000000000005</v>
+      </c>
+      <c r="C18">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>204</v>
+      </c>
+      <c r="B19">
+        <v>478.63</v>
+      </c>
+      <c r="C19">
+        <v>126</v>
+      </c>
+      <c r="D19" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -1403,17 +1655,18 @@
     <hyperlink ref="D10" r:id="rId9" xr:uid="{6F41043D-F05A-E24D-94BF-89A71EBAA506}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E92E4109-F6B1-E946-A2B9-5737B2D369DB}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView zoomScale="212" zoomScaleNormal="212" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" sqref="A1:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1423,19 +1676,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
         <v>115</v>
       </c>
-      <c r="B1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C1" t="s">
-        <v>117</v>
-      </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
@@ -1443,7 +1696,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1457,13 +1710,13 @@
       <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1477,13 +1730,13 @@
       <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -1497,13 +1750,13 @@
       <c r="E4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>162</v>
+      <c r="F4" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -1517,13 +1770,13 @@
       <c r="E5" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1537,16 +1790,16 @@
       <c r="E6" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>216.86</v>
@@ -1557,13 +1810,13 @@
       <c r="E7" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>11</v>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -1577,16 +1830,16 @@
       <c r="E8" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>12</v>
+      <c r="F8" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
       <c r="C9">
         <v>253.6</v>
@@ -1597,13 +1850,13 @@
       <c r="E9" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>14</v>
+      <c r="F9" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -1617,13 +1870,13 @@
       <c r="E10" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>15</v>
+      <c r="F10" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -1638,12 +1891,12 @@
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -1658,15 +1911,15 @@
         <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
       <c r="C13">
         <v>438.17</v>
@@ -1678,12 +1931,12 @@
         <v>4</v>
       </c>
       <c r="F13" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
@@ -1698,12 +1951,12 @@
         <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -1718,12 +1971,12 @@
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -1737,8 +1990,68 @@
       <c r="E16" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>173</v>
+      <c r="F16" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>206</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>454.66</v>
+      </c>
+      <c r="D17">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>208</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>209.99</v>
+      </c>
+      <c r="D18">
+        <v>27</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>211</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>895.55</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -1776,33 +2089,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" t="s">
         <v>115</v>
       </c>
-      <c r="B1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D1" t="s">
-        <v>117</v>
-      </c>
       <c r="E1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F1" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
         <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
       </c>
       <c r="D2">
         <v>105.63</v>
@@ -1810,19 +2123,19 @@
       <c r="E2">
         <v>427</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>28</v>
+      <c r="F2" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
         <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
       </c>
       <c r="D3">
         <v>199.64</v>
@@ -1831,18 +2144,18 @@
         <v>69</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D4">
         <v>160.93</v>
@@ -1851,18 +2164,18 @@
         <v>109</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5">
         <v>260.12</v>
@@ -1871,18 +2184,18 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D6">
         <v>361.87</v>
@@ -1891,18 +2204,18 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D7">
         <v>188.84</v>
@@ -1911,18 +2224,18 @@
         <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8">
         <v>99.55</v>
@@ -1931,18 +2244,18 @@
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D9">
         <v>129.99</v>
@@ -1951,18 +2264,18 @@
         <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10">
         <v>64.98</v>
@@ -1971,7 +2284,7 @@
         <v>162</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2003,22 +2316,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" t="s">
         <v>115</v>
       </c>
-      <c r="B1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>116</v>
-      </c>
-      <c r="D1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" t="s">
-        <v>118</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -2026,16 +2339,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>68</v>
-      </c>
-      <c r="C2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" t="s">
-        <v>70</v>
       </c>
       <c r="E2">
         <v>79.98</v>
@@ -2044,21 +2357,21 @@
         <v>365</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
         <v>72</v>
-      </c>
-      <c r="B3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" t="s">
-        <v>74</v>
       </c>
       <c r="E3">
         <v>159.99</v>
@@ -2067,21 +2380,21 @@
         <v>83</v>
       </c>
       <c r="G3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
         <v>76</v>
-      </c>
-      <c r="B4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" t="s">
-        <v>78</v>
       </c>
       <c r="E4">
         <v>49.99</v>
@@ -2090,21 +2403,21 @@
         <v>688</v>
       </c>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E5">
         <v>159.99</v>
@@ -2113,21 +2426,21 @@
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E6">
         <v>129.97</v>
@@ -2136,21 +2449,21 @@
         <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E7">
         <v>49.99</v>
@@ -2159,21 +2472,21 @@
         <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
         <v>67</v>
       </c>
-      <c r="B8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" t="s">
-        <v>69</v>
-      </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E8">
         <v>58.22</v>
@@ -2182,21 +2495,21 @@
         <v>212</v>
       </c>
       <c r="G8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E9">
         <v>499.99</v>
@@ -2205,21 +2518,21 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E10">
         <v>399.99</v>
@@ -2228,7 +2541,7 @@
         <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2253,16 +2566,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" t="s">
         <v>115</v>
       </c>
-      <c r="B1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C1" t="s">
-        <v>117</v>
-      </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -2270,7 +2583,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -2282,12 +2595,12 @@
         <v>216</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -2299,12 +2612,12 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -2316,12 +2629,12 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -2333,12 +2646,12 @@
         <v>111</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -2350,12 +2663,12 @@
         <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -2367,12 +2680,12 @@
         <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -2384,12 +2697,12 @@
         <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -2401,12 +2714,12 @@
         <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -2418,7 +2731,7 @@
         <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2445,16 +2758,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" t="s">
         <v>115</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>116</v>
-      </c>
-      <c r="C1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D1" t="s">
-        <v>118</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -2462,10 +2775,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C2">
         <v>85.02</v>
@@ -2474,15 +2787,15 @@
         <v>240</v>
       </c>
       <c r="E2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C3">
         <v>99.9</v>
@@ -2491,15 +2804,15 @@
         <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C4">
         <v>89.9</v>
@@ -2508,15 +2821,15 @@
         <v>154</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C5">
         <v>104.94</v>
@@ -2525,15 +2838,15 @@
         <v>155</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C6">
         <v>34.99</v>
@@ -2542,15 +2855,15 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C7">
         <v>200</v>
@@ -2559,15 +2872,15 @@
         <v>79</v>
       </c>
       <c r="E7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C8">
         <v>149.99</v>
@@ -2576,15 +2889,15 @@
         <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C9">
         <v>19.98</v>
@@ -2593,15 +2906,15 @@
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C10">
         <v>289.99</v>
@@ -2610,7 +2923,7 @@
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>